<commit_message>
Update Resume Nov 2024
</commit_message>
<xml_diff>
--- a/data/education_detail.xlsx
+++ b/data/education_detail.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuan Le\Desktop\CV Builder\tuan_le_khac_cv_validus\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuan Le\git\lktuan-resume\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6611DF-DB45-445A-AB38-14488D647837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB8A61-0D4B-4843-99FD-F395071DD7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>eduid</t>
   </si>
@@ -46,6 +58,9 @@
   </si>
   <si>
     <t>GPA: 8.4/10 (3.41/4);</t>
+  </si>
+  <si>
+    <t>GPA: 3.41/4</t>
   </si>
 </sst>
 </file>
@@ -81,8 +96,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,12 +390,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="95.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -386,24 +410,75 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A7DB92-4465-4AEF-ADE3-08660823B5EC}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="95.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>